<commit_message>
agregar -1 para los sin turno en .py y excel
</commit_message>
<xml_diff>
--- a/assets/asistencia/TurnosGeovictoria.xlsx
+++ b/assets/asistencia/TurnosGeovictoria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JMELGAREJO\PythonDevs\10 Asistencia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31D465A-9C26-4EB4-89B9-D0EC373BF54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FEA6BA-16D1-410A-8FA2-8331AC7E0114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4115C1EB-1FF5-4BEC-96A1-7EDCDB37F2F0}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Turno_Lista</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>Turno:  2030-530</t>
+  </si>
+  <si>
+    <t>SinTurno</t>
+  </si>
+  <si>
+    <t>-1</t>
   </si>
 </sst>
 </file>
@@ -605,7 +611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A585DF1-B0AF-42F4-85EA-9B78F3D4152E}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -810,7 +818,12 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>

</xml_diff>